<commit_message>
Import ELSET from Excel file
add import ELSET tool (Material, Section, and Design) from excel file
</commit_message>
<xml_diff>
--- a/Tool_support_reaction_to_pointload_2a.xlsx
+++ b/Tool_support_reaction_to_pointload_2a.xlsx
@@ -8,14 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\COMPUTATIONAL\Python\SANSPRO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C7B1CB3-DF65-4116-A2FA-4A3560532EB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD80E7EA-6498-436B-97AD-043BFB49F153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5ADE9C6B-C934-4942-9032-B82A26DED840}"/>
   </bookViews>
   <sheets>
     <sheet name="Node" sheetId="2" r:id="rId1"/>
     <sheet name="PointLoads" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">PointLoads!$D$3:$D$53</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="1">PointLoads!$AB$3</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +42,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -59,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="43">
   <si>
     <t>index</t>
   </si>
@@ -652,7 +657,7 @@
   <dimension ref="A1:L75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1951,15 +1956,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0FCDDF1-8695-4FC9-AD23-C38011B478F7}">
-  <dimension ref="A1:Z59"/>
+  <dimension ref="A1:AB59"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="AE19" sqref="AE19"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="AB3" sqref="AB3:AB13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="Q1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1973,7 +1978,7 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="Q2" s="3" t="s">
         <v>12</v>
       </c>
@@ -2005,7 +2010,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2075,8 +2080,11 @@
       <c r="Z3" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AB3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2157,8 +2165,11 @@
       <c r="Z4" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AB4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -2239,8 +2250,11 @@
       <c r="Z5" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AB5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -2321,8 +2335,11 @@
       <c r="Z6" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AB6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -2403,8 +2420,11 @@
       <c r="Z7" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AB7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
@@ -2485,8 +2505,11 @@
       <c r="Z8" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AB8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
@@ -2561,8 +2584,11 @@
       <c r="Z9" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AB9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
@@ -2637,8 +2663,11 @@
       <c r="Z10" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AB10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
@@ -2713,8 +2742,11 @@
       <c r="Z11" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AB11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
@@ -2789,8 +2821,11 @@
       <c r="Z12" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AB12">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
@@ -2865,8 +2900,11 @@
       <c r="Z13" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AB13">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>11</v>
       </c>
@@ -2942,7 +2980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12</v>
       </c>
@@ -3018,7 +3056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>13</v>
       </c>
@@ -5981,4 +6019,18 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75F4B754-23E1-4A5C-B04E-CD47CEB31E50}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>